<commit_message>
31-01-2025 country specific analysis
</commit_message>
<xml_diff>
--- a/analysis/results/Q1/beta_diversity/beta_diversity_results_colon.xlsx
+++ b/analysis/results/Q1/beta_diversity/beta_diversity_results_colon.xlsx
@@ -9,6 +9,71 @@
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">pairs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SumsOfSqs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F.Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre_ltx vs healthy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre_ltx vs post_ltx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post_ltx vs healthy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre_ltx vs healthy , Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre_ltx vs post_ltx , Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post_ltx vs healthy , Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre_ltx vs healthy : Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">pre_ltx vs post_ltx : Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post_ltx vs healthy : Country</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,7 +402,268 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1222.92106840471</v>
+      </c>
+      <c r="D2" t="n">
+        <v>7.94994650341597</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0187887705818079</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>630.146146437502</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.06180919840911</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.00662047049736794</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1736.16873682658</v>
+      </c>
+      <c r="D4" t="n">
+        <v>11.0135363130856</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0207805893668765</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>738.576413458271</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4.80132620769844</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0113473740441028</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1532.67469153163</v>
+      </c>
+      <c r="D6" t="n">
+        <v>9.8793465538545</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.016102657510029</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1728.7458235653</v>
+      </c>
+      <c r="D7" t="n">
+        <v>10.9664484217891</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0206917428687702</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>318.719016026873</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.07739496027165</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.00489674977960781</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.325</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.4875</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>322.405182713765</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2.08193228651677</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.00338726819551645</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>398.820084185802</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2.53760726113271</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.00477356620064291</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.112</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.336</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>